<commit_message>
modified logic for centering and moving forward
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BW7"/>
+  <dimension ref="A1:ED7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,144 +659,371 @@
       <c r="BW1" s="1" t="n">
         <v>74</v>
       </c>
+      <c r="BX1" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="BY1" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="BZ1" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="CA1" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="CB1" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="CC1" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="CD1" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="CE1" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="CH1" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="CJ1" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="CK1" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="CP1" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="CQ1" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="CR1" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="CS1" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="CT1" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="CU1" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="CV1" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="CW1" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="CX1" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="CY1" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="CZ1" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="DA1" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="DB1" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="DC1" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="DD1" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="DE1" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="DF1" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="DG1" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="DH1" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="DI1" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="DJ1" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="DK1" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="DL1" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="DM1" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="DN1" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="DO1" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="DP1" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="DQ1" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="DR1" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="DS1" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="DT1" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="DU1" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="DV1" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="DW1" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="DX1" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="DY1" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="DZ1" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="EA1" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="EB1" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="EC1" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="ED1" s="1" t="n">
+        <v>133</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2519386112689972</v>
+        <v>165</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2516157329082489</v>
+        <v>166</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2540744543075562</v>
+        <v>166</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2573143839836121</v>
+        <v>166</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2605262398719788</v>
+        <v>166</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2636201083660126</v>
+        <v>168</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2654843330383301</v>
+        <v>162</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2681801915168762</v>
+        <v>161</v>
       </c>
       <c r="I2" t="n">
-        <v>0.2709054946899414</v>
+        <v>164</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2734079957008362</v>
+        <v>166</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2747969925403595</v>
+        <v>166</v>
       </c>
       <c r="L2" t="n">
-        <v>0.2768981754779816</v>
+        <v>170</v>
       </c>
       <c r="M2" t="n">
-        <v>0.2777315378189087</v>
+        <v>169</v>
       </c>
       <c r="N2" t="n">
-        <v>0.277992457151413</v>
+        <v>166</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2786356806755066</v>
+        <v>169</v>
       </c>
       <c r="P2" t="n">
-        <v>0.279121458530426</v>
+        <v>171</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.2802577018737793</v>
+        <v>170</v>
       </c>
       <c r="R2" t="n">
-        <v>0.2807115018367767</v>
+        <v>170</v>
       </c>
       <c r="S2" t="n">
-        <v>0.2806976735591888</v>
+        <v>170</v>
       </c>
       <c r="T2" t="n">
-        <v>0.2803556621074677</v>
+        <v>165</v>
       </c>
       <c r="U2" t="n">
-        <v>0.2793202996253967</v>
+        <v>164</v>
       </c>
       <c r="V2" t="n">
-        <v>0.2776158154010773</v>
+        <v>171</v>
       </c>
       <c r="W2" t="n">
-        <v>0.2750687301158905</v>
+        <v>170</v>
       </c>
       <c r="X2" t="n">
-        <v>0.273189514875412</v>
+        <v>169</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.2713135182857513</v>
+        <v>169</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.2695842683315277</v>
+        <v>173</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.266521155834198</v>
+        <v>174</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.2650855481624603</v>
+        <v>179</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.2634275555610657</v>
+        <v>179</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.2625400424003601</v>
+        <v>176</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.2612301111221313</v>
+        <v>178</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.2600041329860687</v>
+        <v>179</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.2584095895290375</v>
+        <v>178</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.2567811608314514</v>
+        <v>178</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.2549636960029602</v>
+        <v>179</v>
       </c>
       <c r="AJ2" t="n">
-        <v>0.253271609544754</v>
+        <v>180</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.2511321604251862</v>
-      </c>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr"/>
-      <c r="AV2" t="inlineStr"/>
-      <c r="AW2" t="inlineStr"/>
-      <c r="AX2" t="inlineStr"/>
-      <c r="AY2" t="inlineStr"/>
-      <c r="AZ2" t="inlineStr"/>
-      <c r="BA2" t="inlineStr"/>
-      <c r="BB2" t="inlineStr"/>
-      <c r="BC2" t="inlineStr"/>
-      <c r="BD2" t="inlineStr"/>
-      <c r="BE2" t="inlineStr"/>
-      <c r="BF2" t="inlineStr"/>
-      <c r="BG2" t="inlineStr"/>
-      <c r="BH2" t="inlineStr"/>
-      <c r="BI2" t="inlineStr"/>
-      <c r="BJ2" t="inlineStr"/>
+        <v>176</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>176</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>177</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>172</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>169</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>168</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>168</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>168</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>163</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>164</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>165</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>162</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>162</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>164</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>164</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>165</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>163</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>164</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>165</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>164</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>168</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>164</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>169</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>168</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>165</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>173</v>
+      </c>
       <c r="BK2" t="inlineStr"/>
       <c r="BL2" t="inlineStr"/>
       <c r="BM2" t="inlineStr"/>
@@ -810,522 +1037,917 @@
       <c r="BU2" t="inlineStr"/>
       <c r="BV2" t="inlineStr"/>
       <c r="BW2" t="inlineStr"/>
+      <c r="BX2" t="inlineStr"/>
+      <c r="BY2" t="inlineStr"/>
+      <c r="BZ2" t="inlineStr"/>
+      <c r="CA2" t="inlineStr"/>
+      <c r="CB2" t="inlineStr"/>
+      <c r="CC2" t="inlineStr"/>
+      <c r="CD2" t="inlineStr"/>
+      <c r="CE2" t="inlineStr"/>
+      <c r="CF2" t="inlineStr"/>
+      <c r="CG2" t="inlineStr"/>
+      <c r="CH2" t="inlineStr"/>
+      <c r="CI2" t="inlineStr"/>
+      <c r="CJ2" t="inlineStr"/>
+      <c r="CK2" t="inlineStr"/>
+      <c r="CL2" t="inlineStr"/>
+      <c r="CM2" t="inlineStr"/>
+      <c r="CN2" t="inlineStr"/>
+      <c r="CO2" t="inlineStr"/>
+      <c r="CP2" t="inlineStr"/>
+      <c r="CQ2" t="inlineStr"/>
+      <c r="CR2" t="inlineStr"/>
+      <c r="CS2" t="inlineStr"/>
+      <c r="CT2" t="inlineStr"/>
+      <c r="CU2" t="inlineStr"/>
+      <c r="CV2" t="inlineStr"/>
+      <c r="CW2" t="inlineStr"/>
+      <c r="CX2" t="inlineStr"/>
+      <c r="CY2" t="inlineStr"/>
+      <c r="CZ2" t="inlineStr"/>
+      <c r="DA2" t="inlineStr"/>
+      <c r="DB2" t="inlineStr"/>
+      <c r="DC2" t="inlineStr"/>
+      <c r="DD2" t="inlineStr"/>
+      <c r="DE2" t="inlineStr"/>
+      <c r="DF2" t="inlineStr"/>
+      <c r="DG2" t="inlineStr"/>
+      <c r="DH2" t="inlineStr"/>
+      <c r="DI2" t="inlineStr"/>
+      <c r="DJ2" t="inlineStr"/>
+      <c r="DK2" t="inlineStr"/>
+      <c r="DL2" t="inlineStr"/>
+      <c r="DM2" t="inlineStr"/>
+      <c r="DN2" t="inlineStr"/>
+      <c r="DO2" t="inlineStr"/>
+      <c r="DP2" t="inlineStr"/>
+      <c r="DQ2" t="inlineStr"/>
+      <c r="DR2" t="inlineStr"/>
+      <c r="DS2" t="inlineStr"/>
+      <c r="DT2" t="inlineStr"/>
+      <c r="DU2" t="inlineStr"/>
+      <c r="DV2" t="inlineStr"/>
+      <c r="DW2" t="inlineStr"/>
+      <c r="DX2" t="inlineStr"/>
+      <c r="DY2" t="inlineStr"/>
+      <c r="DZ2" t="inlineStr"/>
+      <c r="EA2" t="inlineStr"/>
+      <c r="EB2" t="inlineStr"/>
+      <c r="EC2" t="inlineStr"/>
+      <c r="ED2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-98.95527648925781</v>
+        <v>15201484300</v>
       </c>
       <c r="B3" t="n">
-        <v>-98.79095458984375</v>
+        <v>15201484300</v>
       </c>
       <c r="C3" t="n">
-        <v>-99.11671447753906</v>
+        <v>22355397500</v>
       </c>
       <c r="D3" t="n">
-        <v>-93.33601379394531</v>
+        <v>22355397500</v>
       </c>
       <c r="E3" t="n">
-        <v>-87.55870056152344</v>
+        <v>22457131500</v>
       </c>
       <c r="F3" t="n">
-        <v>-80.0460205078125</v>
+        <v>22457131500</v>
       </c>
       <c r="G3" t="n">
-        <v>-71.64971923828125</v>
+        <v>22554892300</v>
       </c>
       <c r="H3" t="n">
-        <v>-66.18669128417969</v>
+        <v>22554892300</v>
       </c>
       <c r="I3" t="n">
-        <v>-56.78070068359375</v>
+        <v>22654487300</v>
       </c>
       <c r="J3" t="n">
-        <v>-49.51638793945312</v>
+        <v>22654487300</v>
       </c>
       <c r="K3" t="n">
-        <v>-41.70304870605469</v>
+        <v>22732101400</v>
       </c>
       <c r="L3" t="n">
-        <v>-36.14878845214844</v>
+        <v>22732101400</v>
       </c>
       <c r="M3" t="n">
-        <v>-29.675048828125</v>
+        <v>22805391500</v>
       </c>
       <c r="N3" t="n">
-        <v>-23.21568298339844</v>
+        <v>22805391500</v>
       </c>
       <c r="O3" t="n">
-        <v>-14.80706787109375</v>
+        <v>22883044600</v>
       </c>
       <c r="P3" t="n">
-        <v>-11.84002685546875</v>
+        <v>22883044600</v>
       </c>
       <c r="Q3" t="n">
-        <v>-6.760696411132812</v>
+        <v>22956567400</v>
       </c>
       <c r="R3" t="n">
-        <v>-6.454986572265625</v>
+        <v>22956567400</v>
       </c>
       <c r="S3" t="n">
-        <v>-3.8516845703125</v>
+        <v>23035471900</v>
       </c>
       <c r="T3" t="n">
-        <v>-0.98699951171875</v>
+        <v>23035471900</v>
       </c>
       <c r="U3" t="n">
-        <v>6.992874145507812</v>
+        <v>23109679400</v>
       </c>
       <c r="V3" t="n">
-        <v>7.704833984375</v>
+        <v>23109679400</v>
       </c>
       <c r="W3" t="n">
-        <v>6.627334594726562</v>
+        <v>23185465700</v>
       </c>
       <c r="X3" t="n">
-        <v>6.708251953125</v>
+        <v>23185465700</v>
       </c>
       <c r="Y3" t="n">
-        <v>1.59075927734375</v>
+        <v>23259712300</v>
       </c>
       <c r="Z3" t="n">
-        <v>1.108734130859375</v>
+        <v>23259712300</v>
       </c>
       <c r="AA3" t="n">
-        <v>-5.615447998046875</v>
+        <v>23333415400</v>
       </c>
       <c r="AB3" t="n">
-        <v>-5.238845825195312</v>
+        <v>23333415400</v>
       </c>
       <c r="AC3" t="n">
-        <v>-4.446243286132812</v>
+        <v>23408569700</v>
       </c>
       <c r="AD3" t="n">
-        <v>-3.282501220703125</v>
+        <v>23408569700</v>
       </c>
       <c r="AE3" t="n">
-        <v>-1.361343383789062</v>
+        <v>23485316800</v>
       </c>
       <c r="AF3" t="n">
-        <v>-1.99261474609375</v>
+        <v>23485316800</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.288116455078125</v>
+        <v>23561314100</v>
       </c>
       <c r="AH3" t="n">
-        <v>3.097488403320312</v>
+        <v>23561314100</v>
       </c>
       <c r="AI3" t="n">
-        <v>3.775604248046875</v>
+        <v>23632049300</v>
       </c>
       <c r="AJ3" t="n">
-        <v>4.43402099609375</v>
+        <v>23632049300</v>
       </c>
       <c r="AK3" t="n">
-        <v>4.022125244140625</v>
-      </c>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="inlineStr"/>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="inlineStr"/>
-      <c r="AV3" t="inlineStr"/>
-      <c r="AW3" t="inlineStr"/>
-      <c r="AX3" t="inlineStr"/>
-      <c r="AY3" t="inlineStr"/>
-      <c r="AZ3" t="inlineStr"/>
-      <c r="BA3" t="inlineStr"/>
-      <c r="BB3" t="inlineStr"/>
-      <c r="BC3" t="inlineStr"/>
-      <c r="BD3" t="inlineStr"/>
-      <c r="BE3" t="inlineStr"/>
-      <c r="BF3" t="inlineStr"/>
-      <c r="BG3" t="inlineStr"/>
-      <c r="BH3" t="inlineStr"/>
-      <c r="BI3" t="inlineStr"/>
-      <c r="BJ3" t="inlineStr"/>
-      <c r="BK3" t="inlineStr"/>
-      <c r="BL3" t="inlineStr"/>
-      <c r="BM3" t="inlineStr"/>
-      <c r="BN3" t="inlineStr"/>
-      <c r="BO3" t="inlineStr"/>
-      <c r="BP3" t="inlineStr"/>
-      <c r="BQ3" t="inlineStr"/>
-      <c r="BR3" t="inlineStr"/>
-      <c r="BS3" t="inlineStr"/>
-      <c r="BT3" t="inlineStr"/>
-      <c r="BU3" t="inlineStr"/>
-      <c r="BV3" t="inlineStr"/>
-      <c r="BW3" t="inlineStr"/>
+        <v>23706744500</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>23706744500</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>23783722400</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>23783722400</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>23855151900</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>23855151900</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>23905829300</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>23905829300</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>23978238700</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>23978238700</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>24056063900</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>24056063900</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>24129134300</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>24129134300</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>24180954100</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>24180954100</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>24255932400</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>24255932400</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>24357622200</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>24357622200</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>24407487000</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>24407487000</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>24502632000</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>24502632000</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>24556478700</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>24556478700</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>24628882900</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>24628882900</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>24680352300</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>24680352300</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>24755318600</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>24755318600</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>24804598800</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>24804598800</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>24880316200</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>24880316200</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>24957789100</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>24957789100</v>
+      </c>
+      <c r="BW3" t="n">
+        <v>25031452500</v>
+      </c>
+      <c r="BX3" t="n">
+        <v>25031452500</v>
+      </c>
+      <c r="BY3" t="n">
+        <v>25104411400</v>
+      </c>
+      <c r="BZ3" t="n">
+        <v>25104411400</v>
+      </c>
+      <c r="CA3" t="n">
+        <v>25182289800</v>
+      </c>
+      <c r="CB3" t="n">
+        <v>25182289800</v>
+      </c>
+      <c r="CC3" t="n">
+        <v>25255247300</v>
+      </c>
+      <c r="CD3" t="n">
+        <v>25279640500</v>
+      </c>
+      <c r="CE3" t="n">
+        <v>25303223100</v>
+      </c>
+      <c r="CF3" t="n">
+        <v>25327628700</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>25327628700</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>25379585000</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>25379585000</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>25456856400</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>25503567900</v>
+      </c>
+      <c r="CL3" t="n">
+        <v>25503567900</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>25559574700</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>25559574700</v>
+      </c>
+      <c r="CO3" t="n">
+        <v>25629025300</v>
+      </c>
+      <c r="CP3" t="n">
+        <v>25629025300</v>
+      </c>
+      <c r="CQ3" t="n">
+        <v>25708498900</v>
+      </c>
+      <c r="CR3" t="n">
+        <v>25708498900</v>
+      </c>
+      <c r="CS3" t="n">
+        <v>25780854400</v>
+      </c>
+      <c r="CT3" t="n">
+        <v>25780854400</v>
+      </c>
+      <c r="CU3" t="n">
+        <v>25859257700</v>
+      </c>
+      <c r="CV3" t="n">
+        <v>25903375700</v>
+      </c>
+      <c r="CW3" t="n">
+        <v>25928137600</v>
+      </c>
+      <c r="CX3" t="n">
+        <v>25928137600</v>
+      </c>
+      <c r="CY3" t="n">
+        <v>25979618200</v>
+      </c>
+      <c r="CZ3" t="n">
+        <v>25979618200</v>
+      </c>
+      <c r="DA3" t="n">
+        <v>26028316000</v>
+      </c>
+      <c r="DB3" t="n">
+        <v>26028316000</v>
+      </c>
+      <c r="DC3" t="n">
+        <v>26106623400</v>
+      </c>
+      <c r="DD3" t="n">
+        <v>26153732100</v>
+      </c>
+      <c r="DE3" t="n">
+        <v>26153732100</v>
+      </c>
+      <c r="DF3" t="n">
+        <v>26203548100</v>
+      </c>
+      <c r="DG3" t="n">
+        <v>26203548100</v>
+      </c>
+      <c r="DH3" t="n">
+        <v>26280424900</v>
+      </c>
+      <c r="DI3" t="n">
+        <v>26280424900</v>
+      </c>
+      <c r="DJ3" t="n">
+        <v>26357225400</v>
+      </c>
+      <c r="DK3" t="n">
+        <v>26357225400</v>
+      </c>
+      <c r="DL3" t="n">
+        <v>26429743000</v>
+      </c>
+      <c r="DM3" t="n">
+        <v>26429743000</v>
+      </c>
+      <c r="DN3" t="n">
+        <v>26503919300</v>
+      </c>
+      <c r="DO3" t="n">
+        <v>26503919300</v>
+      </c>
+      <c r="DP3" t="n">
+        <v>26583835100</v>
+      </c>
+      <c r="DQ3" t="n">
+        <v>26583835100</v>
+      </c>
+      <c r="DR3" t="n">
+        <v>26658495400</v>
+      </c>
+      <c r="DS3" t="n">
+        <v>26658495400</v>
+      </c>
+      <c r="DT3" t="n">
+        <v>26729144000</v>
+      </c>
+      <c r="DU3" t="n">
+        <v>26729144000</v>
+      </c>
+      <c r="DV3" t="n">
+        <v>26782674100</v>
+      </c>
+      <c r="DW3" t="n">
+        <v>26782674100</v>
+      </c>
+      <c r="DX3" t="n">
+        <v>26858394400</v>
+      </c>
+      <c r="DY3" t="n">
+        <v>26858394400</v>
+      </c>
+      <c r="DZ3" t="n">
+        <v>26929284500</v>
+      </c>
+      <c r="EA3" t="n">
+        <v>26957395900</v>
+      </c>
+      <c r="EB3" t="n">
+        <v>26978471800</v>
+      </c>
+      <c r="EC3" t="n">
+        <v>26978471800</v>
+      </c>
+      <c r="ED3" t="n">
+        <v>45679765400</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15595981400</v>
+        <v>-0.06720110774040222</v>
       </c>
       <c r="B4" t="n">
-        <v>15595981400</v>
+        <v>-0.06718271970748901</v>
       </c>
       <c r="C4" t="n">
-        <v>20867353800</v>
+        <v>-0.06497882306575775</v>
       </c>
       <c r="D4" t="n">
-        <v>20867353800</v>
+        <v>-0.06353011727333069</v>
       </c>
       <c r="E4" t="n">
-        <v>20993183800</v>
+        <v>-0.06214963644742966</v>
       </c>
       <c r="F4" t="n">
-        <v>20993183800</v>
+        <v>-0.06048240885138512</v>
       </c>
       <c r="G4" t="n">
-        <v>21119688000</v>
+        <v>-0.05885873734951019</v>
       </c>
       <c r="H4" t="n">
-        <v>21119688000</v>
+        <v>-0.05708670988678932</v>
       </c>
       <c r="I4" t="n">
-        <v>21252316800</v>
+        <v>-0.05548758804798126</v>
       </c>
       <c r="J4" t="n">
-        <v>21252316800</v>
+        <v>-0.05404796078801155</v>
       </c>
       <c r="K4" t="n">
-        <v>21395562500</v>
+        <v>-0.05267718434333801</v>
       </c>
       <c r="L4" t="n">
-        <v>21395562500</v>
+        <v>-0.05132760852575302</v>
       </c>
       <c r="M4" t="n">
-        <v>21543560000</v>
+        <v>-0.04942374303936958</v>
       </c>
       <c r="N4" t="n">
-        <v>21543560000</v>
+        <v>-0.04755027964711189</v>
       </c>
       <c r="O4" t="n">
-        <v>21671741500</v>
+        <v>-0.04684571176767349</v>
       </c>
       <c r="P4" t="n">
-        <v>21671741500</v>
+        <v>-0.04501465708017349</v>
       </c>
       <c r="Q4" t="n">
-        <v>21821167500</v>
+        <v>-0.04333491250872612</v>
       </c>
       <c r="R4" t="n">
-        <v>21821167500</v>
+        <v>-0.04229025915265083</v>
       </c>
       <c r="S4" t="n">
-        <v>21946602600</v>
+        <v>-0.0404517650604248</v>
       </c>
       <c r="T4" t="n">
-        <v>21946602600</v>
+        <v>-0.03906914964318275</v>
       </c>
       <c r="U4" t="n">
-        <v>22097574700</v>
+        <v>-0.03877962380647659</v>
       </c>
       <c r="V4" t="n">
-        <v>22097574700</v>
+        <v>-0.03733726590871811</v>
       </c>
       <c r="W4" t="n">
-        <v>22221471600</v>
+        <v>-0.0359986275434494</v>
       </c>
       <c r="X4" t="n">
-        <v>22221471600</v>
+        <v>-0.03531033545732498</v>
       </c>
       <c r="Y4" t="n">
-        <v>22347270000</v>
+        <v>-0.03488509729504585</v>
       </c>
       <c r="Z4" t="n">
-        <v>22347270000</v>
+        <v>-0.03433183953166008</v>
       </c>
       <c r="AA4" t="n">
-        <v>22494442100</v>
+        <v>-0.03371895104646683</v>
       </c>
       <c r="AB4" t="n">
-        <v>22494442100</v>
+        <v>-0.03272360563278198</v>
       </c>
       <c r="AC4" t="n">
-        <v>22619301800</v>
+        <v>-0.03175978362560272</v>
       </c>
       <c r="AD4" t="n">
-        <v>22619301800</v>
+        <v>-0.03189410641789436</v>
       </c>
       <c r="AE4" t="n">
-        <v>22745220400</v>
+        <v>-0.03141331672668457</v>
       </c>
       <c r="AF4" t="n">
-        <v>22745220400</v>
+        <v>-0.03142134472727776</v>
       </c>
       <c r="AG4" t="n">
-        <v>22893944100</v>
+        <v>-0.03211979568004608</v>
       </c>
       <c r="AH4" t="n">
-        <v>22893944100</v>
+        <v>-0.03192878887057304</v>
       </c>
       <c r="AI4" t="n">
-        <v>23050593100</v>
+        <v>-0.0327688492834568</v>
       </c>
       <c r="AJ4" t="n">
-        <v>23050593100</v>
+        <v>-0.03255334496498108</v>
       </c>
       <c r="AK4" t="n">
-        <v>23173087200</v>
+        <v>-0.03317791596055031</v>
       </c>
       <c r="AL4" t="n">
-        <v>23173087200</v>
+        <v>-0.03331988304853439</v>
       </c>
       <c r="AM4" t="n">
-        <v>23320875600</v>
+        <v>-0.03354266285896301</v>
       </c>
       <c r="AN4" t="n">
-        <v>23320875600</v>
+        <v>-0.03331611305475235</v>
       </c>
       <c r="AO4" t="n">
-        <v>23474775700</v>
+        <v>-0.03304215520620346</v>
       </c>
       <c r="AP4" t="n">
-        <v>23474775700</v>
+        <v>-0.03350671753287315</v>
       </c>
       <c r="AQ4" t="n">
-        <v>23594289200</v>
+        <v>-0.03276959806680679</v>
       </c>
       <c r="AR4" t="n">
-        <v>23594289200</v>
+        <v>-0.03242017701268196</v>
       </c>
       <c r="AS4" t="n">
-        <v>23721232500</v>
+        <v>-0.03216175734996796</v>
       </c>
       <c r="AT4" t="n">
-        <v>23721232500</v>
+        <v>-0.03183135390281677</v>
       </c>
       <c r="AU4" t="n">
-        <v>23870851400</v>
+        <v>-0.03151310235261917</v>
       </c>
       <c r="AV4" t="n">
-        <v>23870851400</v>
+        <v>-0.03182894736528397</v>
       </c>
       <c r="AW4" t="n">
-        <v>23994465600</v>
+        <v>-0.03162236884236336</v>
       </c>
       <c r="AX4" t="n">
-        <v>23994465600</v>
+        <v>-0.03140698745846748</v>
       </c>
       <c r="AY4" t="n">
-        <v>24120238600</v>
+        <v>-0.03091935068368912</v>
       </c>
       <c r="AZ4" t="n">
-        <v>24120238600</v>
+        <v>-0.03036525286734104</v>
       </c>
       <c r="BA4" t="n">
-        <v>24247129000</v>
+        <v>-0.03012701496481895</v>
       </c>
       <c r="BB4" t="n">
-        <v>24247129000</v>
+        <v>-0.02985655888915062</v>
       </c>
       <c r="BC4" t="n">
-        <v>24394209700</v>
+        <v>-0.0296211950480938</v>
       </c>
       <c r="BD4" t="n">
-        <v>24394209700</v>
+        <v>-0.02993934229016304</v>
       </c>
       <c r="BE4" t="n">
-        <v>24520448300</v>
+        <v>-0.02979977056384087</v>
       </c>
       <c r="BF4" t="n">
-        <v>24520448300</v>
+        <v>-0.02992848306894302</v>
       </c>
       <c r="BG4" t="n">
-        <v>24674530500</v>
+        <v>-0.02981439791619778</v>
       </c>
       <c r="BH4" t="n">
-        <v>24674530500</v>
+        <v>-0.03040638566017151</v>
       </c>
       <c r="BI4" t="n">
-        <v>24820884900</v>
+        <v>-0.02961792051792145</v>
       </c>
       <c r="BJ4" t="n">
-        <v>24820884900</v>
-      </c>
-      <c r="BK4" t="n">
-        <v>24951141600</v>
-      </c>
-      <c r="BL4" t="n">
-        <v>24951141600</v>
-      </c>
-      <c r="BM4" t="n">
-        <v>25095929800</v>
-      </c>
-      <c r="BN4" t="n">
-        <v>25095929800</v>
-      </c>
-      <c r="BO4" t="n">
-        <v>25250090100</v>
-      </c>
-      <c r="BP4" t="n">
-        <v>25250090100</v>
-      </c>
-      <c r="BQ4" t="n">
-        <v>25370711000</v>
-      </c>
-      <c r="BR4" t="n">
-        <v>25370711000</v>
-      </c>
-      <c r="BS4" t="n">
-        <v>25494308400</v>
-      </c>
-      <c r="BT4" t="n">
-        <v>25494308400</v>
-      </c>
-      <c r="BU4" t="n">
-        <v>25620929600</v>
-      </c>
-      <c r="BV4" t="n">
-        <v>25620929600</v>
-      </c>
-      <c r="BW4" t="n">
-        <v>37314976600</v>
-      </c>
+        <v>-0.02956259064376354</v>
+      </c>
+      <c r="BK4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr"/>
+      <c r="BM4" t="inlineStr"/>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr"/>
+      <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
+      <c r="BS4" t="inlineStr"/>
+      <c r="BT4" t="inlineStr"/>
+      <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="inlineStr"/>
+      <c r="BW4" t="inlineStr"/>
+      <c r="BX4" t="inlineStr"/>
+      <c r="BY4" t="inlineStr"/>
+      <c r="BZ4" t="inlineStr"/>
+      <c r="CA4" t="inlineStr"/>
+      <c r="CB4" t="inlineStr"/>
+      <c r="CC4" t="inlineStr"/>
+      <c r="CD4" t="inlineStr"/>
+      <c r="CE4" t="inlineStr"/>
+      <c r="CF4" t="inlineStr"/>
+      <c r="CG4" t="inlineStr"/>
+      <c r="CH4" t="inlineStr"/>
+      <c r="CI4" t="inlineStr"/>
+      <c r="CJ4" t="inlineStr"/>
+      <c r="CK4" t="inlineStr"/>
+      <c r="CL4" t="inlineStr"/>
+      <c r="CM4" t="inlineStr"/>
+      <c r="CN4" t="inlineStr"/>
+      <c r="CO4" t="inlineStr"/>
+      <c r="CP4" t="inlineStr"/>
+      <c r="CQ4" t="inlineStr"/>
+      <c r="CR4" t="inlineStr"/>
+      <c r="CS4" t="inlineStr"/>
+      <c r="CT4" t="inlineStr"/>
+      <c r="CU4" t="inlineStr"/>
+      <c r="CV4" t="inlineStr"/>
+      <c r="CW4" t="inlineStr"/>
+      <c r="CX4" t="inlineStr"/>
+      <c r="CY4" t="inlineStr"/>
+      <c r="CZ4" t="inlineStr"/>
+      <c r="DA4" t="inlineStr"/>
+      <c r="DB4" t="inlineStr"/>
+      <c r="DC4" t="inlineStr"/>
+      <c r="DD4" t="inlineStr"/>
+      <c r="DE4" t="inlineStr"/>
+      <c r="DF4" t="inlineStr"/>
+      <c r="DG4" t="inlineStr"/>
+      <c r="DH4" t="inlineStr"/>
+      <c r="DI4" t="inlineStr"/>
+      <c r="DJ4" t="inlineStr"/>
+      <c r="DK4" t="inlineStr"/>
+      <c r="DL4" t="inlineStr"/>
+      <c r="DM4" t="inlineStr"/>
+      <c r="DN4" t="inlineStr"/>
+      <c r="DO4" t="inlineStr"/>
+      <c r="DP4" t="inlineStr"/>
+      <c r="DQ4" t="inlineStr"/>
+      <c r="DR4" t="inlineStr"/>
+      <c r="DS4" t="inlineStr"/>
+      <c r="DT4" t="inlineStr"/>
+      <c r="DU4" t="inlineStr"/>
+      <c r="DV4" t="inlineStr"/>
+      <c r="DW4" t="inlineStr"/>
+      <c r="DX4" t="inlineStr"/>
+      <c r="DY4" t="inlineStr"/>
+      <c r="DZ4" t="inlineStr"/>
+      <c r="EA4" t="inlineStr"/>
+      <c r="EB4" t="inlineStr"/>
+      <c r="EC4" t="inlineStr"/>
+      <c r="ED4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>32.23365020751953</v>
+        <v>-109</v>
       </c>
       <c r="B5" t="n">
-        <v>32.04366302490234</v>
+        <v>-110</v>
       </c>
       <c r="C5" t="n">
-        <v>32.12419128417969</v>
+        <v>-109</v>
       </c>
       <c r="D5" t="n">
-        <v>36.15589904785156</v>
+        <v>-105</v>
       </c>
       <c r="E5" t="n">
-        <v>45.63063049316406</v>
+        <v>-97</v>
       </c>
       <c r="F5" t="n">
-        <v>56.48452758789062</v>
+        <v>-90</v>
       </c>
       <c r="G5" t="n">
-        <v>63.14196014404297</v>
+        <v>-91</v>
       </c>
       <c r="H5" t="n">
-        <v>66.42198181152344</v>
+        <v>-87</v>
       </c>
       <c r="I5" t="n">
-        <v>68.56146240234375</v>
+        <v>-78</v>
       </c>
       <c r="J5" t="n">
-        <v>78.897705078125</v>
+        <v>-70</v>
       </c>
       <c r="K5" t="n">
-        <v>82.79550933837891</v>
+        <v>-65</v>
       </c>
       <c r="L5" t="n">
-        <v>88.07826232910156</v>
+        <v>-62</v>
       </c>
       <c r="M5" t="n">
-        <v>91.93059539794922</v>
+        <v>-54</v>
       </c>
       <c r="N5" t="n">
-        <v>94.19544982910156</v>
+        <v>-54</v>
       </c>
       <c r="O5" t="n">
-        <v>97.18813323974609</v>
+        <v>-45</v>
       </c>
       <c r="P5" t="n">
-        <v>96.67725372314453</v>
+        <v>-41</v>
       </c>
       <c r="Q5" t="n">
-        <v>106.8213043212891</v>
+        <v>-38</v>
       </c>
       <c r="R5" t="n">
-        <v>114.2893829345703</v>
+        <v>-29</v>
       </c>
       <c r="S5" t="n">
-        <v>121.4481353759766</v>
+        <v>-23</v>
       </c>
       <c r="T5" t="n">
-        <v>127.9636535644531</v>
+        <v>-25</v>
       </c>
       <c r="U5" t="n">
-        <v>134.6334228515625</v>
+        <v>-17</v>
       </c>
       <c r="V5" t="n">
-        <v>133.0333557128906</v>
+        <v>-11</v>
       </c>
       <c r="W5" t="n">
-        <v>135.4592590332031</v>
+        <v>-9</v>
       </c>
       <c r="X5" t="n">
-        <v>133.7672576904297</v>
+        <v>-4</v>
       </c>
       <c r="Y5" t="n">
-        <v>130.8534088134766</v>
+        <v>-1</v>
       </c>
       <c r="Z5" t="n">
-        <v>125.0146789550781</v>
+        <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>121.0762329101562</v>
+        <v>0</v>
       </c>
       <c r="AB5" t="n">
-        <v>115.4263687133789</v>
+        <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>116.4385452270508</v>
+        <v>2</v>
       </c>
       <c r="AD5" t="n">
-        <v>119.0005569458008</v>
+        <v>9</v>
       </c>
       <c r="AE5" t="n">
-        <v>123.1458053588867</v>
+        <v>10</v>
       </c>
       <c r="AF5" t="n">
-        <v>124.4818649291992</v>
+        <v>12</v>
       </c>
       <c r="AG5" t="n">
-        <v>126.2023162841797</v>
+        <v>11</v>
       </c>
       <c r="AH5" t="n">
-        <v>128.7391967773438</v>
+        <v>10</v>
       </c>
       <c r="AI5" t="n">
-        <v>128.6546478271484</v>
+        <v>10</v>
       </c>
       <c r="AJ5" t="n">
-        <v>127.9653472900391</v>
+        <v>6</v>
       </c>
       <c r="AK5" t="n">
-        <v>127.7789916992188</v>
-      </c>
-      <c r="AL5" t="inlineStr"/>
-      <c r="AM5" t="inlineStr"/>
-      <c r="AN5" t="inlineStr"/>
-      <c r="AO5" t="inlineStr"/>
-      <c r="AP5" t="inlineStr"/>
-      <c r="AQ5" t="inlineStr"/>
-      <c r="AR5" t="inlineStr"/>
-      <c r="AS5" t="inlineStr"/>
-      <c r="AT5" t="inlineStr"/>
-      <c r="AU5" t="inlineStr"/>
-      <c r="AV5" t="inlineStr"/>
-      <c r="AW5" t="inlineStr"/>
-      <c r="AX5" t="inlineStr"/>
-      <c r="AY5" t="inlineStr"/>
-      <c r="AZ5" t="inlineStr"/>
-      <c r="BA5" t="inlineStr"/>
-      <c r="BB5" t="inlineStr"/>
-      <c r="BC5" t="inlineStr"/>
-      <c r="BD5" t="inlineStr"/>
-      <c r="BE5" t="inlineStr"/>
-      <c r="BF5" t="inlineStr"/>
-      <c r="BG5" t="inlineStr"/>
-      <c r="BH5" t="inlineStr"/>
-      <c r="BI5" t="inlineStr"/>
-      <c r="BJ5" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>-4</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>-5</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>-4</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>-4</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>4</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>4</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>3</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>2</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>2</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>4</v>
+      </c>
       <c r="BK5" t="inlineStr"/>
       <c r="BL5" t="inlineStr"/>
       <c r="BM5" t="inlineStr"/>
@@ -1339,144 +1961,253 @@
       <c r="BU5" t="inlineStr"/>
       <c r="BV5" t="inlineStr"/>
       <c r="BW5" t="inlineStr"/>
+      <c r="BX5" t="inlineStr"/>
+      <c r="BY5" t="inlineStr"/>
+      <c r="BZ5" t="inlineStr"/>
+      <c r="CA5" t="inlineStr"/>
+      <c r="CB5" t="inlineStr"/>
+      <c r="CC5" t="inlineStr"/>
+      <c r="CD5" t="inlineStr"/>
+      <c r="CE5" t="inlineStr"/>
+      <c r="CF5" t="inlineStr"/>
+      <c r="CG5" t="inlineStr"/>
+      <c r="CH5" t="inlineStr"/>
+      <c r="CI5" t="inlineStr"/>
+      <c r="CJ5" t="inlineStr"/>
+      <c r="CK5" t="inlineStr"/>
+      <c r="CL5" t="inlineStr"/>
+      <c r="CM5" t="inlineStr"/>
+      <c r="CN5" t="inlineStr"/>
+      <c r="CO5" t="inlineStr"/>
+      <c r="CP5" t="inlineStr"/>
+      <c r="CQ5" t="inlineStr"/>
+      <c r="CR5" t="inlineStr"/>
+      <c r="CS5" t="inlineStr"/>
+      <c r="CT5" t="inlineStr"/>
+      <c r="CU5" t="inlineStr"/>
+      <c r="CV5" t="inlineStr"/>
+      <c r="CW5" t="inlineStr"/>
+      <c r="CX5" t="inlineStr"/>
+      <c r="CY5" t="inlineStr"/>
+      <c r="CZ5" t="inlineStr"/>
+      <c r="DA5" t="inlineStr"/>
+      <c r="DB5" t="inlineStr"/>
+      <c r="DC5" t="inlineStr"/>
+      <c r="DD5" t="inlineStr"/>
+      <c r="DE5" t="inlineStr"/>
+      <c r="DF5" t="inlineStr"/>
+      <c r="DG5" t="inlineStr"/>
+      <c r="DH5" t="inlineStr"/>
+      <c r="DI5" t="inlineStr"/>
+      <c r="DJ5" t="inlineStr"/>
+      <c r="DK5" t="inlineStr"/>
+      <c r="DL5" t="inlineStr"/>
+      <c r="DM5" t="inlineStr"/>
+      <c r="DN5" t="inlineStr"/>
+      <c r="DO5" t="inlineStr"/>
+      <c r="DP5" t="inlineStr"/>
+      <c r="DQ5" t="inlineStr"/>
+      <c r="DR5" t="inlineStr"/>
+      <c r="DS5" t="inlineStr"/>
+      <c r="DT5" t="inlineStr"/>
+      <c r="DU5" t="inlineStr"/>
+      <c r="DV5" t="inlineStr"/>
+      <c r="DW5" t="inlineStr"/>
+      <c r="DX5" t="inlineStr"/>
+      <c r="DY5" t="inlineStr"/>
+      <c r="DZ5" t="inlineStr"/>
+      <c r="EA5" t="inlineStr"/>
+      <c r="EB5" t="inlineStr"/>
+      <c r="EC5" t="inlineStr"/>
+      <c r="ED5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>-0.06708239018917084</v>
+        <v>0.3739813268184662</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.06703667342662811</v>
+        <v>0.3739755153656006</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.06539388746023178</v>
+        <v>0.3743130564689636</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.06320344656705856</v>
+        <v>0.374310314655304</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.05977629497647285</v>
+        <v>0.373788595199585</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.05643238127231598</v>
+        <v>0.3738513886928558</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.05359625816345215</v>
+        <v>0.3737967014312744</v>
       </c>
       <c r="H6" t="n">
-        <v>-0.05082008615136147</v>
+        <v>0.3739155530929565</v>
       </c>
       <c r="I6" t="n">
-        <v>-0.04768969491124153</v>
+        <v>0.3738724291324615</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.04467609524726868</v>
+        <v>0.3738689720630646</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.04264836013317108</v>
+        <v>0.3738954663276672</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.04015214368700981</v>
+        <v>0.3738088309764862</v>
       </c>
       <c r="M6" t="n">
-        <v>-0.03702753782272339</v>
+        <v>0.3739687502384186</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.03482354804873466</v>
+        <v>0.3740731477737427</v>
       </c>
       <c r="O6" t="n">
-        <v>-0.03331748396158218</v>
+        <v>0.3737903237342834</v>
       </c>
       <c r="P6" t="n">
-        <v>-0.03078706376254559</v>
+        <v>0.3734771609306335</v>
       </c>
       <c r="Q6" t="n">
-        <v>-0.02912295237183571</v>
+        <v>0.3735491037368774</v>
       </c>
       <c r="R6" t="n">
-        <v>-0.02736855670809746</v>
+        <v>0.3732628226280212</v>
       </c>
       <c r="S6" t="n">
-        <v>-0.02600026875734329</v>
+        <v>0.3731488883495331</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.02414732612669468</v>
+        <v>0.3736484050750732</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.02334744855761528</v>
+        <v>0.3752704858779907</v>
       </c>
       <c r="V6" t="n">
-        <v>-0.02376093342900276</v>
+        <v>0.3784445524215698</v>
       </c>
       <c r="W6" t="n">
-        <v>-0.02417442761361599</v>
+        <v>0.3823016881942749</v>
       </c>
       <c r="X6" t="n">
-        <v>-0.02432762831449509</v>
+        <v>0.3859825134277344</v>
       </c>
       <c r="Y6" t="n">
-        <v>-0.02537610754370689</v>
+        <v>0.388710081577301</v>
       </c>
       <c r="Z6" t="n">
-        <v>-0.0259439293295145</v>
+        <v>0.3925480842590332</v>
       </c>
       <c r="AA6" t="n">
-        <v>-0.02633979171514511</v>
+        <v>0.3964223861694336</v>
       </c>
       <c r="AB6" t="n">
-        <v>-0.02558890171349049</v>
+        <v>0.4002657532691956</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.02516459859907627</v>
+        <v>0.4055301249027252</v>
       </c>
       <c r="AD6" t="n">
-        <v>-0.02412639558315277</v>
+        <v>0.4079287648200989</v>
       </c>
       <c r="AE6" t="n">
-        <v>-0.02350109443068504</v>
+        <v>0.4119032025337219</v>
       </c>
       <c r="AF6" t="n">
-        <v>-0.02252572402358055</v>
+        <v>0.4143714606761932</v>
       </c>
       <c r="AG6" t="n">
-        <v>-0.02187545970082283</v>
+        <v>0.4181153774261475</v>
       </c>
       <c r="AH6" t="n">
-        <v>-0.0214136615395546</v>
+        <v>0.4206231832504272</v>
       </c>
       <c r="AI6" t="n">
-        <v>-0.0215267539024353</v>
+        <v>0.4243350028991699</v>
       </c>
       <c r="AJ6" t="n">
-        <v>-0.02043025009334087</v>
+        <v>0.4283239245414734</v>
       </c>
       <c r="AK6" t="n">
-        <v>-0.02057889476418495</v>
-      </c>
-      <c r="AL6" t="inlineStr"/>
-      <c r="AM6" t="inlineStr"/>
-      <c r="AN6" t="inlineStr"/>
-      <c r="AO6" t="inlineStr"/>
-      <c r="AP6" t="inlineStr"/>
-      <c r="AQ6" t="inlineStr"/>
-      <c r="AR6" t="inlineStr"/>
-      <c r="AS6" t="inlineStr"/>
-      <c r="AT6" t="inlineStr"/>
-      <c r="AU6" t="inlineStr"/>
-      <c r="AV6" t="inlineStr"/>
-      <c r="AW6" t="inlineStr"/>
-      <c r="AX6" t="inlineStr"/>
-      <c r="AY6" t="inlineStr"/>
-      <c r="AZ6" t="inlineStr"/>
-      <c r="BA6" t="inlineStr"/>
-      <c r="BB6" t="inlineStr"/>
-      <c r="BC6" t="inlineStr"/>
-      <c r="BD6" t="inlineStr"/>
-      <c r="BE6" t="inlineStr"/>
-      <c r="BF6" t="inlineStr"/>
-      <c r="BG6" t="inlineStr"/>
-      <c r="BH6" t="inlineStr"/>
-      <c r="BI6" t="inlineStr"/>
-      <c r="BJ6" t="inlineStr"/>
+        <v>0.4319959282875061</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.4356778264045715</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.4394553899765015</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.4432176351547241</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.449164867401123</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.4510177671909332</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.4539130032062531</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>0.4564604163169861</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>0.4589914679527283</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.4621025323867798</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.4656412601470947</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.4716031849384308</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.4735667109489441</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.4754316210746765</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.4795267581939697</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.4817052781581879</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>0.4850673675537109</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>0.4882178902626038</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>0.4918638467788696</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>0.4942744076251984</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>0.4992163181304932</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>0.503014862537384</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>0.505401611328125</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>0.509161114692688</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>0.513154923915863</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>0.5180075764656067</v>
+      </c>
       <c r="BK6" t="inlineStr"/>
       <c r="BL6" t="inlineStr"/>
       <c r="BM6" t="inlineStr"/>
@@ -1490,144 +2221,253 @@
       <c r="BU6" t="inlineStr"/>
       <c r="BV6" t="inlineStr"/>
       <c r="BW6" t="inlineStr"/>
+      <c r="BX6" t="inlineStr"/>
+      <c r="BY6" t="inlineStr"/>
+      <c r="BZ6" t="inlineStr"/>
+      <c r="CA6" t="inlineStr"/>
+      <c r="CB6" t="inlineStr"/>
+      <c r="CC6" t="inlineStr"/>
+      <c r="CD6" t="inlineStr"/>
+      <c r="CE6" t="inlineStr"/>
+      <c r="CF6" t="inlineStr"/>
+      <c r="CG6" t="inlineStr"/>
+      <c r="CH6" t="inlineStr"/>
+      <c r="CI6" t="inlineStr"/>
+      <c r="CJ6" t="inlineStr"/>
+      <c r="CK6" t="inlineStr"/>
+      <c r="CL6" t="inlineStr"/>
+      <c r="CM6" t="inlineStr"/>
+      <c r="CN6" t="inlineStr"/>
+      <c r="CO6" t="inlineStr"/>
+      <c r="CP6" t="inlineStr"/>
+      <c r="CQ6" t="inlineStr"/>
+      <c r="CR6" t="inlineStr"/>
+      <c r="CS6" t="inlineStr"/>
+      <c r="CT6" t="inlineStr"/>
+      <c r="CU6" t="inlineStr"/>
+      <c r="CV6" t="inlineStr"/>
+      <c r="CW6" t="inlineStr"/>
+      <c r="CX6" t="inlineStr"/>
+      <c r="CY6" t="inlineStr"/>
+      <c r="CZ6" t="inlineStr"/>
+      <c r="DA6" t="inlineStr"/>
+      <c r="DB6" t="inlineStr"/>
+      <c r="DC6" t="inlineStr"/>
+      <c r="DD6" t="inlineStr"/>
+      <c r="DE6" t="inlineStr"/>
+      <c r="DF6" t="inlineStr"/>
+      <c r="DG6" t="inlineStr"/>
+      <c r="DH6" t="inlineStr"/>
+      <c r="DI6" t="inlineStr"/>
+      <c r="DJ6" t="inlineStr"/>
+      <c r="DK6" t="inlineStr"/>
+      <c r="DL6" t="inlineStr"/>
+      <c r="DM6" t="inlineStr"/>
+      <c r="DN6" t="inlineStr"/>
+      <c r="DO6" t="inlineStr"/>
+      <c r="DP6" t="inlineStr"/>
+      <c r="DQ6" t="inlineStr"/>
+      <c r="DR6" t="inlineStr"/>
+      <c r="DS6" t="inlineStr"/>
+      <c r="DT6" t="inlineStr"/>
+      <c r="DU6" t="inlineStr"/>
+      <c r="DV6" t="inlineStr"/>
+      <c r="DW6" t="inlineStr"/>
+      <c r="DX6" t="inlineStr"/>
+      <c r="DY6" t="inlineStr"/>
+      <c r="DZ6" t="inlineStr"/>
+      <c r="EA6" t="inlineStr"/>
+      <c r="EB6" t="inlineStr"/>
+      <c r="EC6" t="inlineStr"/>
+      <c r="ED6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.3738492131233215</v>
+        <v>0.2519175112247467</v>
       </c>
       <c r="B7" t="n">
-        <v>0.3738498985767365</v>
+        <v>0.2519148886203766</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3739902973175049</v>
+        <v>0.2519509494304657</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3740625381469727</v>
+        <v>0.2522769570350647</v>
       </c>
       <c r="E7" t="n">
-        <v>0.3742305040359497</v>
+        <v>0.2520036697387695</v>
       </c>
       <c r="F7" t="n">
-        <v>0.3743196129798889</v>
+        <v>0.251908928155899</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3737888932228088</v>
+        <v>0.2525860667228699</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3733679354190826</v>
+        <v>0.2526797354221344</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3733852505683899</v>
+        <v>0.2527430653572083</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3731854259967804</v>
+        <v>0.2531038224697113</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3728930354118347</v>
+        <v>0.2535432875156403</v>
       </c>
       <c r="L7" t="n">
-        <v>0.3727410733699799</v>
+        <v>0.2539354264736176</v>
       </c>
       <c r="M7" t="n">
-        <v>0.3726773262023926</v>
+        <v>0.2540239095687866</v>
       </c>
       <c r="N7" t="n">
-        <v>0.3727008998394012</v>
+        <v>0.2539981305599213</v>
       </c>
       <c r="O7" t="n">
-        <v>0.3763855695724487</v>
+        <v>0.2537488341331482</v>
       </c>
       <c r="P7" t="n">
-        <v>0.3837035298347473</v>
+        <v>0.2542527914047241</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.3915847539901733</v>
+        <v>0.2542939782142639</v>
       </c>
       <c r="R7" t="n">
-        <v>0.3979745507240295</v>
+        <v>0.2539733648300171</v>
       </c>
       <c r="S7" t="n">
-        <v>0.4056183695793152</v>
+        <v>0.2537637054920197</v>
       </c>
       <c r="T7" t="n">
-        <v>0.413306713104248</v>
+        <v>0.2538881897926331</v>
       </c>
       <c r="U7" t="n">
-        <v>0.4196228384971619</v>
+        <v>0.2543507218360901</v>
       </c>
       <c r="V7" t="n">
-        <v>0.4251996874809265</v>
+        <v>0.2542030513286591</v>
       </c>
       <c r="W7" t="n">
-        <v>0.4270835220813751</v>
+        <v>0.2541262209415436</v>
       </c>
       <c r="X7" t="n">
-        <v>0.4273950755596161</v>
+        <v>0.2539441883563995</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.4274955987930298</v>
+        <v>0.2540287673473358</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.4276046752929688</v>
+        <v>0.2540146112442017</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.4283043146133423</v>
+        <v>0.2544302642345428</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.4337136447429657</v>
+        <v>0.2541031241416931</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.4409530162811279</v>
+        <v>0.2542297542095184</v>
       </c>
       <c r="AD7" t="n">
-        <v>0.4486740529537201</v>
+        <v>0.2539677917957306</v>
       </c>
       <c r="AE7" t="n">
-        <v>0.4549288153648376</v>
+        <v>0.2538392841815948</v>
       </c>
       <c r="AF7" t="n">
-        <v>0.4623391926288605</v>
+        <v>0.2536462545394897</v>
       </c>
       <c r="AG7" t="n">
-        <v>0.4699141979217529</v>
+        <v>0.2532103955745697</v>
       </c>
       <c r="AH7" t="n">
-        <v>0.4761449694633484</v>
+        <v>0.2533032894134521</v>
       </c>
       <c r="AI7" t="n">
-        <v>0.4823528826236725</v>
+        <v>0.2528544068336487</v>
       </c>
       <c r="AJ7" t="n">
-        <v>0.4886808395385742</v>
+        <v>0.2525593638420105</v>
       </c>
       <c r="AK7" t="n">
-        <v>0.4961781799793243</v>
-      </c>
-      <c r="AL7" t="inlineStr"/>
-      <c r="AM7" t="inlineStr"/>
-      <c r="AN7" t="inlineStr"/>
-      <c r="AO7" t="inlineStr"/>
-      <c r="AP7" t="inlineStr"/>
-      <c r="AQ7" t="inlineStr"/>
-      <c r="AR7" t="inlineStr"/>
-      <c r="AS7" t="inlineStr"/>
-      <c r="AT7" t="inlineStr"/>
-      <c r="AU7" t="inlineStr"/>
-      <c r="AV7" t="inlineStr"/>
-      <c r="AW7" t="inlineStr"/>
-      <c r="AX7" t="inlineStr"/>
-      <c r="AY7" t="inlineStr"/>
-      <c r="AZ7" t="inlineStr"/>
-      <c r="BA7" t="inlineStr"/>
-      <c r="BB7" t="inlineStr"/>
-      <c r="BC7" t="inlineStr"/>
-      <c r="BD7" t="inlineStr"/>
-      <c r="BE7" t="inlineStr"/>
-      <c r="BF7" t="inlineStr"/>
-      <c r="BG7" t="inlineStr"/>
-      <c r="BH7" t="inlineStr"/>
-      <c r="BI7" t="inlineStr"/>
-      <c r="BJ7" t="inlineStr"/>
+        <v>0.2523325979709625</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0.252156138420105</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0.2516412138938904</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>0.2515429258346558</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>0.2509000599384308</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0.2507681548595428</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0.2512170672416687</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>0.2509549260139465</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>0.2511062324047089</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0.2513051331043243</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.2508113980293274</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>0.2512947916984558</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>0.2513436377048492</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>0.2513790130615234</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>0.2518110871315002</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>0.2519572675228119</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>0.2523297667503357</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>0.2523761093616486</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>0.2524414956569672</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>0.2528014183044434</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>0.2526473701000214</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0.2531695961952209</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>0.2529886662960052</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>0.2531881034374237</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>0.2539108991622925</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0.2535675466060638</v>
+      </c>
       <c r="BK7" t="inlineStr"/>
       <c r="BL7" t="inlineStr"/>
       <c r="BM7" t="inlineStr"/>
@@ -1641,6 +2481,65 @@
       <c r="BU7" t="inlineStr"/>
       <c r="BV7" t="inlineStr"/>
       <c r="BW7" t="inlineStr"/>
+      <c r="BX7" t="inlineStr"/>
+      <c r="BY7" t="inlineStr"/>
+      <c r="BZ7" t="inlineStr"/>
+      <c r="CA7" t="inlineStr"/>
+      <c r="CB7" t="inlineStr"/>
+      <c r="CC7" t="inlineStr"/>
+      <c r="CD7" t="inlineStr"/>
+      <c r="CE7" t="inlineStr"/>
+      <c r="CF7" t="inlineStr"/>
+      <c r="CG7" t="inlineStr"/>
+      <c r="CH7" t="inlineStr"/>
+      <c r="CI7" t="inlineStr"/>
+      <c r="CJ7" t="inlineStr"/>
+      <c r="CK7" t="inlineStr"/>
+      <c r="CL7" t="inlineStr"/>
+      <c r="CM7" t="inlineStr"/>
+      <c r="CN7" t="inlineStr"/>
+      <c r="CO7" t="inlineStr"/>
+      <c r="CP7" t="inlineStr"/>
+      <c r="CQ7" t="inlineStr"/>
+      <c r="CR7" t="inlineStr"/>
+      <c r="CS7" t="inlineStr"/>
+      <c r="CT7" t="inlineStr"/>
+      <c r="CU7" t="inlineStr"/>
+      <c r="CV7" t="inlineStr"/>
+      <c r="CW7" t="inlineStr"/>
+      <c r="CX7" t="inlineStr"/>
+      <c r="CY7" t="inlineStr"/>
+      <c r="CZ7" t="inlineStr"/>
+      <c r="DA7" t="inlineStr"/>
+      <c r="DB7" t="inlineStr"/>
+      <c r="DC7" t="inlineStr"/>
+      <c r="DD7" t="inlineStr"/>
+      <c r="DE7" t="inlineStr"/>
+      <c r="DF7" t="inlineStr"/>
+      <c r="DG7" t="inlineStr"/>
+      <c r="DH7" t="inlineStr"/>
+      <c r="DI7" t="inlineStr"/>
+      <c r="DJ7" t="inlineStr"/>
+      <c r="DK7" t="inlineStr"/>
+      <c r="DL7" t="inlineStr"/>
+      <c r="DM7" t="inlineStr"/>
+      <c r="DN7" t="inlineStr"/>
+      <c r="DO7" t="inlineStr"/>
+      <c r="DP7" t="inlineStr"/>
+      <c r="DQ7" t="inlineStr"/>
+      <c r="DR7" t="inlineStr"/>
+      <c r="DS7" t="inlineStr"/>
+      <c r="DT7" t="inlineStr"/>
+      <c r="DU7" t="inlineStr"/>
+      <c r="DV7" t="inlineStr"/>
+      <c r="DW7" t="inlineStr"/>
+      <c r="DX7" t="inlineStr"/>
+      <c r="DY7" t="inlineStr"/>
+      <c r="DZ7" t="inlineStr"/>
+      <c r="EA7" t="inlineStr"/>
+      <c r="EB7" t="inlineStr"/>
+      <c r="EC7" t="inlineStr"/>
+      <c r="ED7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>